<commit_message>
Fix "Res edit" QC report formatting
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_res_edit.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_res_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37580F50-8E42-4106-B95E-8B924B90352A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4C2AC5-55AB-4A12-97DA-3578551A3ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31800" yWindow="2985" windowWidth="21600" windowHeight="11295" tabRatio="654" xr2:uid="{4FE36DF5-B547-4381-982D-E4288ABB34ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="654" xr2:uid="{4FE36DF5-B547-4381-982D-E4288ABB34ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>PARID</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>2024 Dwelling Total</t>
+  </si>
+  <si>
+    <t>TAXYR</t>
+  </si>
+  <si>
+    <t>TOWNSHIP</t>
   </si>
 </sst>
 </file>
@@ -691,362 +697,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB31AF90-9008-46D8-9D90-08E0DF3D5DB1}">
-  <dimension ref="A1:CD1"/>
+  <dimension ref="A1:CF1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="17" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="15.5703125" customWidth="1"/>
-    <col min="89" max="89" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="8" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="92" max="93" width="11" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="17" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="15.5703125" customWidth="1"/>
+    <col min="91" max="91" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="11" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="11" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BW1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CF1" s="7" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switch current year to prior year on wrong columns
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_res_edit.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_res_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE4EB87-BC7D-4EDD-8024-D89D539F4839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9702E1B-2D52-4A4E-9471-BF8BFB4C9F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35160" yWindow="3765" windowWidth="27765" windowHeight="9525" tabRatio="654" xr2:uid="{4FE36DF5-B547-4381-982D-E4288ABB34ED}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" tabRatio="654" xr2:uid="{4FE36DF5-B547-4381-982D-E4288ABB34ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>PARID</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Prior Year TMV</t>
+  </si>
+  <si>
+    <t>Prior Year Dwelling MV</t>
+  </si>
+  <si>
+    <t>Prior Year Dwelling Total</t>
   </si>
 </sst>
 </file>
@@ -874,10 +880,10 @@
         <v>78</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="6" t="s">
         <v>17</v>

</xml_diff>